<commit_message>
Initial commit for floating projects
</commit_message>
<xml_diff>
--- a/analysis/results/statistics/stats_output.xlsx
+++ b/analysis/results/statistics/stats_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>R2</t>
   </si>
@@ -22,12 +22,21 @@
     <t>Adjusted R2</t>
   </si>
   <si>
+    <t>Experience factor</t>
+  </si>
+  <si>
+    <t>Experience factor standard error</t>
+  </si>
+  <si>
     <t>Learning rate</t>
   </si>
   <si>
     <t>Predictor variable</t>
   </si>
   <si>
+    <t>Coefficient</t>
+  </si>
+  <si>
     <t>P-value</t>
   </si>
   <si>
@@ -40,12 +49,6 @@
     <t>Water Depth Max (m)</t>
   </si>
   <si>
-    <t>Turbine MW (Max)</t>
-  </si>
-  <si>
-    <t>Capacity MW (Max)</t>
-  </si>
-  <si>
     <t>Distance From Shore Auto (km)</t>
   </si>
   <si>
@@ -61,7 +64,7 @@
     <t>Netherlands</t>
   </si>
   <si>
-    <t>Other</t>
+    <t>Denmark</t>
   </si>
   <si>
     <t>log Cumulative Capacity</t>
@@ -396,166 +399,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>0.8429178400431043</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>0.7703480079554758</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.8080106933860164</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>0.7312583071819396</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.0730889024183029</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>-0.1766480063435771</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.04488352281937748</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B5">
+        <v>0.1152437251467398</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>1.687328308428613E-30</v>
-      </c>
-      <c r="C6">
-        <v>294.361383261599</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
-        <v>0.1320066391141676</v>
-      </c>
-      <c r="C7">
-        <v>3.218850589621745</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>0.3092476963872158</v>
+        <v>10.01964084590913</v>
       </c>
       <c r="C8">
-        <v>2.051649808314644</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>7.503085231517034E-30</v>
+      </c>
+      <c r="D8">
+        <v>259.6754510514192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>9.619094652105668E-05</v>
+        <v>0.00243396834500138</v>
       </c>
       <c r="C9">
-        <v>2.347265153952156</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>0.4850095709435859</v>
+      </c>
+      <c r="D9">
+        <v>3.10858594488866</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>0.02038260909948635</v>
+        <v>0.000989679974745061</v>
       </c>
       <c r="C10">
-        <v>1.976601495120095</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>0.3758057699861492</v>
+      </c>
+      <c r="D10">
+        <v>1.769582676427884</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>0.001506957454422182</v>
+        <v>-0.09345311504986542</v>
       </c>
       <c r="C11">
-        <v>3.118663732295853</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>0.2292920911877039</v>
+      </c>
+      <c r="D11">
+        <v>2.38263085379547</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12">
-        <v>3.544498190731757E-09</v>
+        <v>-0.5184750768619801</v>
       </c>
       <c r="C12">
-        <v>5.075110455869929</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>3.898718070655649E-06</v>
+      </c>
+      <c r="D12">
+        <v>3.875755336571895</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>0.0002776290418123979</v>
+        <v>-0.2045210812476508</v>
       </c>
       <c r="C13">
-        <v>1.66009359117456</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>0.05366329404719031</v>
+      </c>
+      <c r="D13">
+        <v>1.278706172593232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>0.3495603497512897</v>
+        <v>-0.1759677541525662</v>
       </c>
       <c r="C14">
-        <v>1.179783788271904</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>0.2017558645641216</v>
+      </c>
+      <c r="D14">
+        <v>1.148672010644807</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>0.00371454164951101</v>
+        <v>-0.4618562439295095</v>
       </c>
       <c r="C15">
-        <v>1.23741072867511</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>0.0219755287161753</v>
+      </c>
+      <c r="D15">
+        <v>1.203169735251236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>0.0196827106581904</v>
+        <v>-0.1766480063435771</v>
       </c>
       <c r="C16">
-        <v>2.113092855911847</v>
+        <v>0.0002725979274128292</v>
+      </c>
+      <c r="D16">
+        <v>1.483881529870047</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-commit after losing conda env
</commit_message>
<xml_diff>
--- a/analysis/results/statistics/stats_output.xlsx
+++ b/analysis/results/statistics/stats_output.xlsx
@@ -426,7 +426,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-0.1766480063435771</v>
+        <v>-0.1766480063435774</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -434,7 +434,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.04488352281937748</v>
+        <v>0.04488352281937752</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -442,7 +442,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.1152437251467398</v>
+        <v>0.11524372514674</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -464,10 +464,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>10.01964084590913</v>
+        <v>10.01964084590914</v>
       </c>
       <c r="C8">
-        <v>7.503085231517034E-30</v>
+        <v>7.50308523151725E-30</v>
       </c>
       <c r="D8">
         <v>259.6754510514192</v>
@@ -478,10 +478,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>0.00243396834500138</v>
+        <v>0.002433968345001678</v>
       </c>
       <c r="C9">
-        <v>0.4850095709435859</v>
+        <v>0.4850095709435331</v>
       </c>
       <c r="D9">
         <v>3.10858594488866</v>
@@ -492,10 +492,10 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>0.000989679974745061</v>
+        <v>0.000989679974744969</v>
       </c>
       <c r="C10">
-        <v>0.3758057699861492</v>
+        <v>0.375805769986193</v>
       </c>
       <c r="D10">
         <v>1.769582676427884</v>
@@ -506,10 +506,10 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>-0.09345311504986542</v>
+        <v>-0.09345311504986409</v>
       </c>
       <c r="C11">
-        <v>0.2292920911877039</v>
+        <v>0.2292920911877105</v>
       </c>
       <c r="D11">
         <v>2.38263085379547</v>
@@ -520,10 +520,10 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>-0.5184750768619801</v>
+        <v>-0.5184750768619794</v>
       </c>
       <c r="C12">
-        <v>3.898718070655649E-06</v>
+        <v>3.898718070655699E-06</v>
       </c>
       <c r="D12">
         <v>3.875755336571895</v>
@@ -534,10 +534,10 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>-0.2045210812476508</v>
+        <v>-0.2045210812476517</v>
       </c>
       <c r="C13">
-        <v>0.05366329404719031</v>
+        <v>0.0536632940471894</v>
       </c>
       <c r="D13">
         <v>1.278706172593232</v>
@@ -548,10 +548,10 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>-0.1759677541525662</v>
+        <v>-0.1759677541525635</v>
       </c>
       <c r="C14">
-        <v>0.2017558645641216</v>
+        <v>0.2017558645641281</v>
       </c>
       <c r="D14">
         <v>1.148672010644807</v>
@@ -565,7 +565,7 @@
         <v>-0.4618562439295095</v>
       </c>
       <c r="C15">
-        <v>0.0219755287161753</v>
+        <v>0.02197552871617524</v>
       </c>
       <c r="D15">
         <v>1.203169735251236</v>
@@ -576,10 +576,10 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>-0.1766480063435771</v>
+        <v>-0.1766480063435774</v>
       </c>
       <c r="C16">
-        <v>0.0002725979274128292</v>
+        <v>0.0002725979274128266</v>
       </c>
       <c r="D16">
         <v>1.483881529870047</v>

</xml_diff>

<commit_message>
Updates for report revision
</commit_message>
<xml_diff>
--- a/analysis/results/statistics/stats_output.xlsx
+++ b/analysis/results/statistics/stats_output.xlsx
@@ -426,7 +426,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-0.1766480063435771</v>
+        <v>-0.1766480063435774</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -434,7 +434,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.04488352281937748</v>
+        <v>0.04488352281937752</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -442,7 +442,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.1152437251467398</v>
+        <v>0.11524372514674</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -464,10 +464,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>10.01964084590913</v>
+        <v>10.01964084590914</v>
       </c>
       <c r="C8">
-        <v>7.503085231517034E-30</v>
+        <v>7.50308523151725E-30</v>
       </c>
       <c r="D8">
         <v>259.6754510514192</v>
@@ -478,10 +478,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>0.00243396834500138</v>
+        <v>0.002433968345001678</v>
       </c>
       <c r="C9">
-        <v>0.4850095709435859</v>
+        <v>0.4850095709435331</v>
       </c>
       <c r="D9">
         <v>3.10858594488866</v>
@@ -492,10 +492,10 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>0.000989679974745061</v>
+        <v>0.000989679974744969</v>
       </c>
       <c r="C10">
-        <v>0.3758057699861492</v>
+        <v>0.375805769986193</v>
       </c>
       <c r="D10">
         <v>1.769582676427884</v>
@@ -506,10 +506,10 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>-0.09345311504986542</v>
+        <v>-0.09345311504986409</v>
       </c>
       <c r="C11">
-        <v>0.2292920911877039</v>
+        <v>0.2292920911877105</v>
       </c>
       <c r="D11">
         <v>2.38263085379547</v>
@@ -520,10 +520,10 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>-0.5184750768619801</v>
+        <v>-0.5184750768619794</v>
       </c>
       <c r="C12">
-        <v>3.898718070655649E-06</v>
+        <v>3.898718070655699E-06</v>
       </c>
       <c r="D12">
         <v>3.875755336571895</v>
@@ -534,10 +534,10 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>-0.2045210812476508</v>
+        <v>-0.2045210812476517</v>
       </c>
       <c r="C13">
-        <v>0.05366329404719031</v>
+        <v>0.0536632940471894</v>
       </c>
       <c r="D13">
         <v>1.278706172593232</v>
@@ -548,10 +548,10 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>-0.1759677541525662</v>
+        <v>-0.1759677541525635</v>
       </c>
       <c r="C14">
-        <v>0.2017558645641216</v>
+        <v>0.2017558645641281</v>
       </c>
       <c r="D14">
         <v>1.148672010644807</v>
@@ -565,7 +565,7 @@
         <v>-0.4618562439295095</v>
       </c>
       <c r="C15">
-        <v>0.0219755287161753</v>
+        <v>0.02197552871617524</v>
       </c>
       <c r="D15">
         <v>1.203169735251236</v>
@@ -576,10 +576,10 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>-0.1766480063435771</v>
+        <v>-0.1766480063435774</v>
       </c>
       <c r="C16">
-        <v>0.0002725979274128292</v>
+        <v>0.0002725979274128266</v>
       </c>
       <c r="D16">
         <v>1.483881529870047</v>

</xml_diff>

<commit_message>
Created alternate waterfall with turbine upsizing shifted to AEP (increase NCF, dont control for turbine size)
</commit_message>
<xml_diff>
--- a/analysis/results/statistics/stats_output.xlsx
+++ b/analysis/results/statistics/stats_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>R2</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Water Depth Max (m)</t>
+  </si>
+  <si>
+    <t>Turbine MW (Max)</t>
   </si>
   <si>
     <t>Distance From Shore Auto (km)</t>
@@ -399,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -410,7 +413,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>0.7703480079554758</v>
+        <v>0.7789394126229221</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -418,7 +421,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.7312583071819396</v>
+        <v>0.7356884281361025</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -426,7 +429,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-0.1766480063435774</v>
+        <v>-0.1394830801295063</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -434,7 +437,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.04488352281937752</v>
+        <v>0.05247784092368975</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -442,7 +445,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.11524372514674</v>
+        <v>0.09215562090148766</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -464,13 +467,13 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>10.01964084590914</v>
+        <v>9.838244731852322</v>
       </c>
       <c r="C8">
-        <v>7.50308523151725E-30</v>
+        <v>4.04585454425828E-28</v>
       </c>
       <c r="D8">
-        <v>259.6754510514192</v>
+        <v>293.4640298004076</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -478,13 +481,13 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>0.002433968345001678</v>
+        <v>0.002256454357066718</v>
       </c>
       <c r="C9">
-        <v>0.4850095709435331</v>
+        <v>0.5141655967132666</v>
       </c>
       <c r="D9">
-        <v>3.10858594488866</v>
+        <v>3.113244435205369</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -492,13 +495,13 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>0.000989679974744969</v>
+        <v>-0.02540563173149829</v>
       </c>
       <c r="C10">
-        <v>0.375805769986193</v>
+        <v>0.1877734100736426</v>
       </c>
       <c r="D10">
-        <v>1.769582676427884</v>
+        <v>2.020394491472369</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -506,13 +509,13 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>-0.09345311504986409</v>
+        <v>0.001008263652520233</v>
       </c>
       <c r="C11">
-        <v>0.2292920911877105</v>
+        <v>0.3631727090827571</v>
       </c>
       <c r="D11">
-        <v>2.38263085379547</v>
+        <v>1.769866376082421</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -520,13 +523,13 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>-0.5184750768619794</v>
+        <v>-0.09671777836262829</v>
       </c>
       <c r="C12">
-        <v>3.898718070655699E-06</v>
+        <v>0.2103138239935414</v>
       </c>
       <c r="D12">
-        <v>3.875755336571895</v>
+        <v>2.385084263250463</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -534,13 +537,13 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>-0.2045210812476517</v>
+        <v>-0.5751835369196083</v>
       </c>
       <c r="C13">
-        <v>0.0536632940471894</v>
+        <v>2.526736984961288E-06</v>
       </c>
       <c r="D13">
-        <v>1.278706172593232</v>
+        <v>4.596016041490434</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -548,13 +551,13 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>-0.1759677541525635</v>
+        <v>-0.1914250922273117</v>
       </c>
       <c r="C14">
-        <v>0.2017558645641281</v>
+        <v>0.06935966836624897</v>
       </c>
       <c r="D14">
-        <v>1.148672010644807</v>
+        <v>1.290387114164369</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -562,13 +565,13 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>-0.4618562439295095</v>
+        <v>-0.186113242206102</v>
       </c>
       <c r="C15">
-        <v>0.02197552871617524</v>
+        <v>0.1746956213269577</v>
       </c>
       <c r="D15">
-        <v>1.203169735251236</v>
+        <v>1.152312062370935</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -576,13 +579,27 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>-0.1766480063435774</v>
+        <v>-0.4300437592982931</v>
       </c>
       <c r="C16">
-        <v>0.0002725979274128266</v>
+        <v>0.03227215930131837</v>
       </c>
       <c r="D16">
-        <v>1.483881529870047</v>
+        <v>1.221395920549448</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>-0.1394830801295063</v>
+      </c>
+      <c r="C17">
+        <v>0.01077644068359378</v>
+      </c>
+      <c r="D17">
+        <v>2.062510387941916</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data_out.  Reverted assumptions back to original waterfall (include turbine upsizing in Capex)
</commit_message>
<xml_diff>
--- a/analysis/results/statistics/stats_output.xlsx
+++ b/analysis/results/statistics/stats_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>R2</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Water Depth Max (m)</t>
-  </si>
-  <si>
-    <t>Turbine MW (Max)</t>
   </si>
   <si>
     <t>Distance From Shore Auto (km)</t>
@@ -402,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -413,7 +410,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>0.7789394126229221</v>
+        <v>0.7703480079554758</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -421,7 +418,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.7356884281361025</v>
+        <v>0.7312583071819396</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -429,7 +426,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-0.1394830801295063</v>
+        <v>-0.1766480063435774</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -437,7 +434,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.05247784092368975</v>
+        <v>0.04488352281937752</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -445,7 +442,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.09215562090148766</v>
+        <v>0.11524372514674</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -467,13 +464,13 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>9.838244731852322</v>
+        <v>10.01964084590914</v>
       </c>
       <c r="C8">
-        <v>4.04585454425828E-28</v>
+        <v>7.50308523151725E-30</v>
       </c>
       <c r="D8">
-        <v>293.4640298004076</v>
+        <v>259.6754510514192</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -481,13 +478,13 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>0.002256454357066718</v>
+        <v>0.002433968345001678</v>
       </c>
       <c r="C9">
-        <v>0.5141655967132666</v>
+        <v>0.4850095709435331</v>
       </c>
       <c r="D9">
-        <v>3.113244435205369</v>
+        <v>3.10858594488866</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -495,13 +492,13 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>-0.02540563173149829</v>
+        <v>0.000989679974744969</v>
       </c>
       <c r="C10">
-        <v>0.1877734100736426</v>
+        <v>0.375805769986193</v>
       </c>
       <c r="D10">
-        <v>2.020394491472369</v>
+        <v>1.769582676427884</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -509,13 +506,13 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>0.001008263652520233</v>
+        <v>-0.09345311504986409</v>
       </c>
       <c r="C11">
-        <v>0.3631727090827571</v>
+        <v>0.2292920911877105</v>
       </c>
       <c r="D11">
-        <v>1.769866376082421</v>
+        <v>2.38263085379547</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -523,13 +520,13 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>-0.09671777836262829</v>
+        <v>-0.5184750768619794</v>
       </c>
       <c r="C12">
-        <v>0.2103138239935414</v>
+        <v>3.898718070655699E-06</v>
       </c>
       <c r="D12">
-        <v>2.385084263250463</v>
+        <v>3.875755336571895</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -537,13 +534,13 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>-0.5751835369196083</v>
+        <v>-0.2045210812476517</v>
       </c>
       <c r="C13">
-        <v>2.526736984961288E-06</v>
+        <v>0.0536632940471894</v>
       </c>
       <c r="D13">
-        <v>4.596016041490434</v>
+        <v>1.278706172593232</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -551,13 +548,13 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>-0.1914250922273117</v>
+        <v>-0.1759677541525635</v>
       </c>
       <c r="C14">
-        <v>0.06935966836624897</v>
+        <v>0.2017558645641281</v>
       </c>
       <c r="D14">
-        <v>1.290387114164369</v>
+        <v>1.148672010644807</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -565,13 +562,13 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>-0.186113242206102</v>
+        <v>-0.4618562439295095</v>
       </c>
       <c r="C15">
-        <v>0.1746956213269577</v>
+        <v>0.02197552871617524</v>
       </c>
       <c r="D15">
-        <v>1.152312062370935</v>
+        <v>1.203169735251236</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -579,27 +576,13 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>-0.4300437592982931</v>
+        <v>-0.1766480063435774</v>
       </c>
       <c r="C16">
-        <v>0.03227215930131837</v>
+        <v>0.0002725979274128266</v>
       </c>
       <c r="D16">
-        <v>1.221395920549448</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17">
-        <v>-0.1394830801295063</v>
-      </c>
-      <c r="C17">
-        <v>0.01077644068359378</v>
-      </c>
-      <c r="D17">
-        <v>2.062510387941916</v>
+        <v>1.483881529870047</v>
       </c>
     </row>
   </sheetData>

</xml_diff>